<commit_message>
filter array in answer
</commit_message>
<xml_diff>
--- a/test_protocol.xlsx
+++ b/test_protocol.xlsx
@@ -1,15 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roman\OneDrive - Северный Арктический Федеральный Университет\MED\FormGenerator\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_A61BBE49BB564791BA1D7E1D1BAF135E528283D1" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{C2F39231-0689-45E8-B2FA-F29AFC74E0C4}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="15180" windowHeight="9345" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ФВД" sheetId="1" r:id="rId1"/>
     <sheet name="проба с бронхолитиком" sheetId="2" r:id="rId2"/>
     <sheet name="проба с физ. нагрузкой" sheetId="3" r:id="rId3"/>
+    <sheet name="Лист1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="92512"/>
 </workbook>
@@ -159,8 +166,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -363,13 +370,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -407,9 +422,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -441,9 +456,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -475,9 +508,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -650,7 +701,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M209"/>
   <sheetViews>
@@ -658,24 +709,24 @@
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10.5"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" style="7" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" style="7" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="8" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" style="9" customWidth="1"/>
-    <col min="5" max="5" width="50.7109375" style="10" customWidth="1"/>
-    <col min="6" max="6" width="70.7109375" style="7" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="7" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" style="7" customWidth="1"/>
-    <col min="9" max="9" width="30.7109375" style="7" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" style="7" customWidth="1"/>
-    <col min="11" max="12" width="20.7109375" style="7" customWidth="1"/>
-    <col min="13" max="13" width="50.7109375" style="7" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="7"/>
+    <col min="2" max="2" width="40.6640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" style="9" customWidth="1"/>
+    <col min="5" max="5" width="50.6640625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="70.6640625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="20.6640625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="30.6640625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" style="7" customWidth="1"/>
+    <col min="11" max="12" width="20.6640625" style="7" customWidth="1"/>
+    <col min="13" max="13" width="50.6640625" style="7" customWidth="1"/>
+    <col min="14" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="5" customFormat="1" ht="12.75">
+    <row r="1" spans="1:13" s="5" customFormat="1" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
@@ -692,7 +743,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="4" spans="1:13" s="9" customFormat="1" ht="21">
+    <row r="4" spans="1:13" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>0</v>
       </c>
@@ -709,7 +760,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>5</v>
       </c>
@@ -718,12 +769,12 @@
       <c r="D5" s="6"/>
       <c r="E5" s="16"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C6" s="15"/>
       <c r="D6" s="6"/>
       <c r="E6" s="16"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>8</v>
       </c>
@@ -737,7 +788,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="21">
+    <row r="8" spans="1:13" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>5</v>
       </c>
@@ -751,7 +802,7 @@
       <c r="E8" s="16"/>
       <c r="F8" s="18"/>
     </row>
-    <row r="9" spans="1:13" ht="21">
+    <row r="9" spans="1:13" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>5</v>
       </c>
@@ -767,7 +818,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>8</v>
       </c>
@@ -778,7 +829,7 @@
       <c r="D10" s="6"/>
       <c r="E10" s="16"/>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
@@ -789,7 +840,7 @@
       <c r="D11" s="6"/>
       <c r="E11" s="16"/>
     </row>
-    <row r="12" spans="1:13" ht="21">
+    <row r="12" spans="1:13" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>5</v>
       </c>
@@ -802,7 +853,7 @@
       <c r="D12" s="6"/>
       <c r="E12" s="16"/>
     </row>
-    <row r="13" spans="1:13" ht="21">
+    <row r="13" spans="1:13" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>5</v>
       </c>
@@ -816,7 +867,7 @@
       <c r="E13" s="16"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:13" ht="21">
+    <row r="14" spans="1:13" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="25" t="s">
         <v>18</v>
@@ -828,7 +879,7 @@
       <c r="E14" s="16"/>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:13" ht="21">
+    <row r="15" spans="1:13" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="15" t="s">
         <v>19</v>
@@ -840,7 +891,7 @@
       <c r="E15" s="16"/>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>5</v>
       </c>
@@ -851,7 +902,7 @@
       <c r="D16" s="6"/>
       <c r="E16" s="16"/>
     </row>
-    <row r="17" spans="1:5" ht="21">
+    <row r="17" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>5</v>
       </c>
@@ -864,7 +915,7 @@
       <c r="D17" s="6"/>
       <c r="E17" s="16"/>
     </row>
-    <row r="18" spans="1:5" ht="21">
+    <row r="18" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
@@ -877,7 +928,7 @@
       <c r="D18" s="6"/>
       <c r="E18" s="16"/>
     </row>
-    <row r="19" spans="1:5" ht="21">
+    <row r="19" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>5</v>
       </c>
@@ -890,7 +941,7 @@
       <c r="D19" s="6"/>
       <c r="E19" s="16"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>5</v>
       </c>
@@ -901,7 +952,7 @@
       <c r="D20" s="6"/>
       <c r="E20" s="16"/>
     </row>
-    <row r="21" spans="1:5" ht="21">
+    <row r="21" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>5</v>
       </c>
@@ -914,7 +965,7 @@
       <c r="D21" s="6"/>
       <c r="E21" s="16"/>
     </row>
-    <row r="22" spans="1:5" ht="21">
+    <row r="22" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>5</v>
       </c>
@@ -931,7 +982,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="21">
+    <row r="23" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="14"/>
       <c r="C23" s="19" t="s">
@@ -940,7 +991,7 @@
       <c r="D23" s="6"/>
       <c r="E23" s="16"/>
     </row>
-    <row r="24" spans="1:5" ht="21">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="14"/>
       <c r="C24" s="15"/>
@@ -949,7 +1000,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="21">
+    <row r="25" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="14"/>
       <c r="C25" s="19" t="s">
@@ -958,7 +1009,7 @@
       <c r="D25" s="6"/>
       <c r="E25" s="16"/>
     </row>
-    <row r="26" spans="1:5" ht="21">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="14"/>
       <c r="C26" s="15"/>
@@ -967,7 +1018,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="21">
+    <row r="27" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>
       <c r="B27" s="14"/>
       <c r="C27" s="19" t="s">
@@ -976,7 +1027,7 @@
       <c r="D27" s="6"/>
       <c r="E27" s="16"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="14"/>
       <c r="B28" s="14"/>
       <c r="C28" s="15"/>
@@ -985,7 +1036,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="21">
+    <row r="29" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
       <c r="B29" s="14"/>
       <c r="C29" s="19" t="s">
@@ -994,77 +1045,77 @@
       <c r="D29" s="6"/>
       <c r="E29" s="16"/>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
       <c r="B30" s="14"/>
       <c r="C30" s="15"/>
       <c r="D30" s="6"/>
       <c r="E30" s="16"/>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="14"/>
       <c r="B31" s="14"/>
       <c r="C31" s="15"/>
       <c r="D31" s="6"/>
       <c r="E31" s="16"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="14"/>
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
       <c r="D32" s="6"/>
       <c r="E32" s="16"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="14"/>
       <c r="B33" s="14"/>
       <c r="C33" s="15"/>
       <c r="D33" s="6"/>
       <c r="E33" s="16"/>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="14"/>
       <c r="B34" s="14"/>
       <c r="C34" s="15"/>
       <c r="D34" s="6"/>
       <c r="E34" s="16"/>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="14"/>
       <c r="B35" s="14"/>
       <c r="C35" s="15"/>
       <c r="D35" s="6"/>
       <c r="E35" s="16"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="14"/>
       <c r="B36" s="14"/>
       <c r="C36" s="15"/>
       <c r="D36" s="6"/>
       <c r="E36" s="16"/>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
       <c r="D37" s="6"/>
       <c r="E37" s="16"/>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="14"/>
       <c r="B38" s="14"/>
       <c r="C38" s="15"/>
       <c r="D38" s="6"/>
       <c r="E38" s="16"/>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="14"/>
       <c r="B39" s="14"/>
       <c r="C39" s="15"/>
       <c r="D39" s="6"/>
       <c r="E39" s="16"/>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="14"/>
       <c r="B40" s="14"/>
       <c r="C40" s="15"/>
@@ -1072,1183 +1123,1183 @@
       <c r="E40" s="16"/>
       <c r="F40" s="22"/>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="14"/>
       <c r="B41" s="14"/>
       <c r="C41" s="21"/>
       <c r="D41" s="6"/>
       <c r="E41" s="16"/>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="14"/>
       <c r="B42" s="14"/>
       <c r="C42" s="15"/>
       <c r="D42" s="6"/>
       <c r="E42" s="16"/>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="14"/>
       <c r="B43" s="14"/>
       <c r="C43" s="15"/>
       <c r="D43" s="6"/>
       <c r="E43" s="16"/>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="14"/>
       <c r="B44" s="14"/>
       <c r="C44" s="15"/>
       <c r="D44" s="6"/>
       <c r="E44" s="16"/>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="14"/>
       <c r="B45" s="14"/>
       <c r="C45" s="15"/>
       <c r="D45" s="6"/>
       <c r="E45" s="16"/>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="14"/>
       <c r="B46" s="14"/>
       <c r="C46" s="15"/>
       <c r="D46" s="6"/>
       <c r="E46" s="16"/>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="14"/>
       <c r="B47" s="14"/>
       <c r="C47" s="15"/>
       <c r="D47" s="6"/>
       <c r="E47" s="16"/>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="14"/>
       <c r="B48" s="14"/>
       <c r="C48" s="15"/>
       <c r="D48" s="6"/>
       <c r="E48" s="16"/>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="14"/>
       <c r="B49" s="14"/>
       <c r="C49" s="15"/>
       <c r="D49" s="6"/>
       <c r="E49" s="16"/>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="14"/>
       <c r="B50" s="14"/>
       <c r="C50" s="15"/>
       <c r="D50" s="6"/>
       <c r="E50" s="16"/>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="14"/>
       <c r="B51" s="14"/>
       <c r="C51" s="15"/>
       <c r="D51" s="6"/>
       <c r="E51" s="16"/>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="14"/>
       <c r="B52" s="14"/>
       <c r="C52" s="15"/>
       <c r="D52" s="6"/>
       <c r="E52" s="16"/>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="14"/>
       <c r="B53" s="14"/>
       <c r="C53" s="15"/>
       <c r="D53" s="6"/>
       <c r="E53" s="16"/>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="14"/>
       <c r="B54" s="14"/>
       <c r="C54" s="15"/>
       <c r="D54" s="6"/>
       <c r="E54" s="16"/>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="14"/>
       <c r="B55" s="14"/>
       <c r="C55" s="15"/>
       <c r="D55" s="6"/>
       <c r="E55" s="16"/>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="14"/>
       <c r="B56" s="14"/>
       <c r="C56" s="15"/>
       <c r="D56" s="6"/>
       <c r="E56" s="16"/>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="14"/>
       <c r="B57" s="14"/>
       <c r="C57" s="15"/>
       <c r="D57" s="6"/>
       <c r="E57" s="16"/>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="14"/>
       <c r="B58" s="14"/>
       <c r="C58" s="15"/>
       <c r="D58" s="6"/>
       <c r="E58" s="16"/>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="14"/>
       <c r="B59" s="14"/>
       <c r="C59" s="15"/>
       <c r="D59" s="6"/>
       <c r="E59" s="16"/>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="14"/>
       <c r="B60" s="14"/>
       <c r="C60" s="15"/>
       <c r="D60" s="6"/>
       <c r="E60" s="16"/>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="14"/>
       <c r="B61" s="14"/>
       <c r="C61" s="15"/>
       <c r="D61" s="6"/>
       <c r="E61" s="16"/>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="14"/>
       <c r="B62" s="14"/>
       <c r="C62" s="15"/>
       <c r="D62" s="6"/>
       <c r="E62" s="16"/>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="14"/>
       <c r="B63" s="14"/>
       <c r="C63" s="15"/>
       <c r="D63" s="6"/>
       <c r="E63" s="16"/>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="14"/>
       <c r="B64" s="14"/>
       <c r="C64" s="15"/>
       <c r="D64" s="6"/>
       <c r="E64" s="16"/>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="14"/>
       <c r="B65" s="14"/>
       <c r="C65" s="15"/>
       <c r="D65" s="6"/>
       <c r="E65" s="16"/>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="14"/>
       <c r="B66" s="14"/>
       <c r="C66" s="15"/>
       <c r="D66" s="6"/>
       <c r="E66" s="16"/>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="14"/>
       <c r="B67" s="14"/>
       <c r="C67" s="15"/>
       <c r="D67" s="6"/>
       <c r="E67" s="16"/>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="14"/>
       <c r="B68" s="14"/>
       <c r="C68" s="15"/>
       <c r="D68" s="6"/>
       <c r="E68" s="16"/>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="14"/>
       <c r="B69" s="14"/>
       <c r="C69" s="15"/>
       <c r="D69" s="6"/>
       <c r="E69" s="16"/>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="14"/>
       <c r="B70" s="14"/>
       <c r="C70" s="15"/>
       <c r="D70" s="6"/>
       <c r="E70" s="16"/>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="14"/>
       <c r="B71" s="14"/>
       <c r="C71" s="15"/>
       <c r="D71" s="6"/>
       <c r="E71" s="16"/>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="14"/>
       <c r="B72" s="14"/>
       <c r="C72" s="15"/>
       <c r="D72" s="6"/>
       <c r="E72" s="16"/>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="14"/>
       <c r="B73" s="14"/>
       <c r="C73" s="15"/>
       <c r="D73" s="6"/>
       <c r="E73" s="16"/>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="14"/>
       <c r="B74" s="14"/>
       <c r="C74" s="15"/>
       <c r="D74" s="6"/>
       <c r="E74" s="16"/>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="14"/>
       <c r="B75" s="14"/>
       <c r="C75" s="15"/>
       <c r="D75" s="6"/>
       <c r="E75" s="16"/>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="14"/>
       <c r="B76" s="14"/>
       <c r="C76" s="15"/>
       <c r="D76" s="6"/>
       <c r="E76" s="16"/>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="14"/>
       <c r="B77" s="14"/>
       <c r="C77" s="15"/>
       <c r="D77" s="6"/>
       <c r="E77" s="16"/>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="14"/>
       <c r="B78" s="14"/>
       <c r="C78" s="15"/>
       <c r="D78" s="6"/>
       <c r="E78" s="16"/>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="14"/>
       <c r="B79" s="14"/>
       <c r="C79" s="15"/>
       <c r="D79" s="6"/>
       <c r="E79" s="16"/>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="14"/>
       <c r="B80" s="14"/>
       <c r="C80" s="15"/>
       <c r="D80" s="6"/>
       <c r="E80" s="16"/>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="14"/>
       <c r="B81" s="14"/>
       <c r="C81" s="15"/>
       <c r="D81" s="6"/>
       <c r="E81" s="16"/>
     </row>
-    <row r="82" spans="1:5">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="14"/>
       <c r="B82" s="14"/>
       <c r="C82" s="15"/>
       <c r="D82" s="6"/>
       <c r="E82" s="16"/>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="14"/>
       <c r="B83" s="14"/>
       <c r="C83" s="15"/>
       <c r="D83" s="6"/>
       <c r="E83" s="16"/>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="14"/>
       <c r="B84" s="14"/>
       <c r="C84" s="15"/>
       <c r="D84" s="6"/>
       <c r="E84" s="16"/>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="14"/>
       <c r="B85" s="14"/>
       <c r="C85" s="15"/>
       <c r="D85" s="6"/>
       <c r="E85" s="16"/>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="14"/>
       <c r="B86" s="14"/>
       <c r="C86" s="15"/>
       <c r="D86" s="6"/>
       <c r="E86" s="16"/>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="14"/>
       <c r="B87" s="14"/>
       <c r="C87" s="15"/>
       <c r="D87" s="6"/>
       <c r="E87" s="16"/>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="14"/>
       <c r="B88" s="14"/>
       <c r="C88" s="15"/>
       <c r="D88" s="6"/>
       <c r="E88" s="16"/>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="14"/>
       <c r="B89" s="14"/>
       <c r="C89" s="15"/>
       <c r="D89" s="6"/>
       <c r="E89" s="16"/>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="14"/>
       <c r="B90" s="14"/>
       <c r="C90" s="15"/>
       <c r="D90" s="6"/>
       <c r="E90" s="16"/>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="14"/>
       <c r="B91" s="14"/>
       <c r="C91" s="15"/>
       <c r="D91" s="6"/>
       <c r="E91" s="16"/>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="14"/>
       <c r="B92" s="14"/>
       <c r="C92" s="15"/>
       <c r="D92" s="6"/>
       <c r="E92" s="16"/>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="14"/>
       <c r="B93" s="14"/>
       <c r="C93" s="15"/>
       <c r="D93" s="6"/>
       <c r="E93" s="16"/>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="14"/>
       <c r="B94" s="14"/>
       <c r="C94" s="15"/>
       <c r="D94" s="6"/>
       <c r="E94" s="16"/>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="14"/>
       <c r="B95" s="14"/>
       <c r="C95" s="15"/>
       <c r="D95" s="6"/>
       <c r="E95" s="16"/>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="14"/>
       <c r="B96" s="14"/>
       <c r="C96" s="15"/>
       <c r="D96" s="6"/>
       <c r="E96" s="16"/>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="14"/>
       <c r="B97" s="14"/>
       <c r="C97" s="15"/>
       <c r="D97" s="6"/>
       <c r="E97" s="16"/>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="14"/>
       <c r="B98" s="14"/>
       <c r="C98" s="15"/>
       <c r="D98" s="6"/>
       <c r="E98" s="16"/>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="14"/>
       <c r="B99" s="14"/>
       <c r="C99" s="15"/>
       <c r="D99" s="6"/>
       <c r="E99" s="16"/>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="14"/>
       <c r="B100" s="14"/>
       <c r="C100" s="15"/>
       <c r="D100" s="6"/>
       <c r="E100" s="16"/>
     </row>
-    <row r="101" spans="1:5">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="14"/>
       <c r="B101" s="14"/>
       <c r="C101" s="15"/>
       <c r="D101" s="6"/>
       <c r="E101" s="16"/>
     </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="14"/>
       <c r="B102" s="14"/>
       <c r="C102" s="15"/>
       <c r="D102" s="6"/>
       <c r="E102" s="16"/>
     </row>
-    <row r="103" spans="1:5">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="14"/>
       <c r="B103" s="14"/>
       <c r="C103" s="15"/>
       <c r="D103" s="6"/>
       <c r="E103" s="16"/>
     </row>
-    <row r="104" spans="1:5">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="14"/>
       <c r="B104" s="14"/>
       <c r="C104" s="15"/>
       <c r="D104" s="6"/>
       <c r="E104" s="16"/>
     </row>
-    <row r="105" spans="1:5">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="14"/>
       <c r="B105" s="14"/>
       <c r="C105" s="15"/>
       <c r="D105" s="6"/>
       <c r="E105" s="16"/>
     </row>
-    <row r="106" spans="1:5">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="14"/>
       <c r="B106" s="14"/>
       <c r="C106" s="15"/>
       <c r="D106" s="6"/>
       <c r="E106" s="16"/>
     </row>
-    <row r="107" spans="1:5">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="14"/>
       <c r="B107" s="14"/>
       <c r="C107" s="15"/>
       <c r="D107" s="6"/>
       <c r="E107" s="16"/>
     </row>
-    <row r="108" spans="1:5">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="14"/>
       <c r="B108" s="14"/>
       <c r="C108" s="15"/>
       <c r="D108" s="6"/>
       <c r="E108" s="16"/>
     </row>
-    <row r="109" spans="1:5">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="14"/>
       <c r="B109" s="14"/>
       <c r="C109" s="15"/>
       <c r="D109" s="6"/>
       <c r="E109" s="16"/>
     </row>
-    <row r="110" spans="1:5">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="14"/>
       <c r="B110" s="14"/>
       <c r="C110" s="15"/>
       <c r="D110" s="6"/>
       <c r="E110" s="16"/>
     </row>
-    <row r="111" spans="1:5">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="14"/>
       <c r="B111" s="14"/>
       <c r="C111" s="15"/>
       <c r="D111" s="6"/>
       <c r="E111" s="16"/>
     </row>
-    <row r="112" spans="1:5">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="14"/>
       <c r="B112" s="14"/>
       <c r="C112" s="15"/>
       <c r="D112" s="6"/>
       <c r="E112" s="16"/>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="14"/>
       <c r="B113" s="14"/>
       <c r="C113" s="15"/>
       <c r="D113" s="6"/>
       <c r="E113" s="16"/>
     </row>
-    <row r="114" spans="1:5">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="14"/>
       <c r="B114" s="14"/>
       <c r="C114" s="15"/>
       <c r="D114" s="6"/>
       <c r="E114" s="16"/>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="14"/>
       <c r="B115" s="14"/>
       <c r="C115" s="15"/>
       <c r="D115" s="6"/>
       <c r="E115" s="16"/>
     </row>
-    <row r="116" spans="1:5">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="14"/>
       <c r="B116" s="14"/>
       <c r="C116" s="15"/>
       <c r="D116" s="6"/>
       <c r="E116" s="16"/>
     </row>
-    <row r="117" spans="1:5">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="14"/>
       <c r="B117" s="14"/>
       <c r="C117" s="15"/>
       <c r="D117" s="6"/>
       <c r="E117" s="16"/>
     </row>
-    <row r="118" spans="1:5">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="14"/>
       <c r="B118" s="14"/>
       <c r="C118" s="15"/>
       <c r="D118" s="6"/>
       <c r="E118" s="16"/>
     </row>
-    <row r="119" spans="1:5">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="14"/>
       <c r="B119" s="14"/>
       <c r="C119" s="15"/>
       <c r="D119" s="6"/>
       <c r="E119" s="16"/>
     </row>
-    <row r="120" spans="1:5">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="14"/>
       <c r="B120" s="14"/>
       <c r="C120" s="15"/>
       <c r="D120" s="6"/>
       <c r="E120" s="16"/>
     </row>
-    <row r="121" spans="1:5">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="14"/>
       <c r="B121" s="14"/>
       <c r="C121" s="15"/>
       <c r="D121" s="6"/>
       <c r="E121" s="16"/>
     </row>
-    <row r="122" spans="1:5">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="14"/>
       <c r="B122" s="14"/>
       <c r="C122" s="15"/>
       <c r="D122" s="6"/>
       <c r="E122" s="16"/>
     </row>
-    <row r="123" spans="1:5">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="14"/>
       <c r="B123" s="14"/>
       <c r="C123" s="15"/>
       <c r="D123" s="6"/>
       <c r="E123" s="16"/>
     </row>
-    <row r="124" spans="1:5">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="14"/>
       <c r="B124" s="14"/>
       <c r="C124" s="15"/>
       <c r="D124" s="6"/>
       <c r="E124" s="16"/>
     </row>
-    <row r="125" spans="1:5">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="14"/>
       <c r="B125" s="14"/>
       <c r="C125" s="15"/>
       <c r="D125" s="6"/>
       <c r="E125" s="16"/>
     </row>
-    <row r="126" spans="1:5">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="14"/>
       <c r="B126" s="14"/>
       <c r="C126" s="15"/>
       <c r="D126" s="6"/>
       <c r="E126" s="16"/>
     </row>
-    <row r="127" spans="1:5">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="14"/>
       <c r="B127" s="14"/>
       <c r="C127" s="15"/>
       <c r="D127" s="6"/>
       <c r="E127" s="16"/>
     </row>
-    <row r="128" spans="1:5">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="14"/>
       <c r="B128" s="14"/>
       <c r="C128" s="15"/>
       <c r="D128" s="6"/>
       <c r="E128" s="16"/>
     </row>
-    <row r="129" spans="1:5">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="14"/>
       <c r="B129" s="14"/>
       <c r="C129" s="15"/>
       <c r="D129" s="6"/>
       <c r="E129" s="16"/>
     </row>
-    <row r="130" spans="1:5">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="14"/>
       <c r="B130" s="14"/>
       <c r="C130" s="15"/>
       <c r="D130" s="6"/>
       <c r="E130" s="16"/>
     </row>
-    <row r="131" spans="1:5">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="14"/>
       <c r="B131" s="14"/>
       <c r="C131" s="15"/>
       <c r="D131" s="6"/>
       <c r="E131" s="16"/>
     </row>
-    <row r="132" spans="1:5">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="14"/>
       <c r="B132" s="14"/>
       <c r="C132" s="15"/>
       <c r="D132" s="6"/>
       <c r="E132" s="16"/>
     </row>
-    <row r="133" spans="1:5">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="14"/>
       <c r="B133" s="14"/>
       <c r="C133" s="15"/>
       <c r="D133" s="6"/>
       <c r="E133" s="16"/>
     </row>
-    <row r="134" spans="1:5">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="14"/>
       <c r="B134" s="14"/>
       <c r="C134" s="15"/>
       <c r="D134" s="6"/>
       <c r="E134" s="16"/>
     </row>
-    <row r="135" spans="1:5">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="14"/>
       <c r="B135" s="14"/>
       <c r="C135" s="15"/>
       <c r="D135" s="6"/>
       <c r="E135" s="16"/>
     </row>
-    <row r="136" spans="1:5">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="14"/>
       <c r="B136" s="14"/>
       <c r="C136" s="15"/>
       <c r="D136" s="6"/>
       <c r="E136" s="16"/>
     </row>
-    <row r="137" spans="1:5">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="14"/>
       <c r="B137" s="14"/>
       <c r="C137" s="15"/>
       <c r="D137" s="6"/>
       <c r="E137" s="16"/>
     </row>
-    <row r="138" spans="1:5">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="14"/>
       <c r="B138" s="14"/>
       <c r="C138" s="15"/>
       <c r="D138" s="6"/>
       <c r="E138" s="16"/>
     </row>
-    <row r="139" spans="1:5">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="14"/>
       <c r="B139" s="14"/>
       <c r="C139" s="15"/>
       <c r="D139" s="6"/>
       <c r="E139" s="16"/>
     </row>
-    <row r="140" spans="1:5">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="14"/>
       <c r="B140" s="14"/>
       <c r="C140" s="15"/>
       <c r="D140" s="6"/>
       <c r="E140" s="16"/>
     </row>
-    <row r="141" spans="1:5">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="14"/>
       <c r="B141" s="14"/>
       <c r="C141" s="15"/>
       <c r="D141" s="6"/>
       <c r="E141" s="16"/>
     </row>
-    <row r="142" spans="1:5">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="14"/>
       <c r="B142" s="14"/>
       <c r="C142" s="15"/>
       <c r="D142" s="6"/>
       <c r="E142" s="16"/>
     </row>
-    <row r="143" spans="1:5">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="14"/>
       <c r="B143" s="14"/>
       <c r="C143" s="15"/>
       <c r="D143" s="6"/>
       <c r="E143" s="16"/>
     </row>
-    <row r="144" spans="1:5">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="14"/>
       <c r="B144" s="14"/>
       <c r="C144" s="15"/>
       <c r="D144" s="6"/>
       <c r="E144" s="16"/>
     </row>
-    <row r="145" spans="1:5">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="14"/>
       <c r="B145" s="14"/>
       <c r="C145" s="15"/>
       <c r="D145" s="6"/>
       <c r="E145" s="16"/>
     </row>
-    <row r="146" spans="1:5">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="14"/>
       <c r="B146" s="14"/>
       <c r="C146" s="15"/>
       <c r="D146" s="6"/>
       <c r="E146" s="16"/>
     </row>
-    <row r="147" spans="1:5">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="14"/>
       <c r="B147" s="14"/>
       <c r="C147" s="15"/>
       <c r="D147" s="6"/>
       <c r="E147" s="16"/>
     </row>
-    <row r="148" spans="1:5">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="14"/>
       <c r="B148" s="14"/>
       <c r="C148" s="15"/>
       <c r="D148" s="6"/>
       <c r="E148" s="16"/>
     </row>
-    <row r="149" spans="1:5">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="14"/>
       <c r="B149" s="14"/>
       <c r="C149" s="15"/>
       <c r="D149" s="6"/>
       <c r="E149" s="16"/>
     </row>
-    <row r="150" spans="1:5">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="14"/>
       <c r="B150" s="14"/>
       <c r="C150" s="15"/>
       <c r="D150" s="6"/>
       <c r="E150" s="16"/>
     </row>
-    <row r="151" spans="1:5">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="14"/>
       <c r="B151" s="14"/>
       <c r="C151" s="15"/>
       <c r="D151" s="6"/>
       <c r="E151" s="16"/>
     </row>
-    <row r="152" spans="1:5">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="14"/>
       <c r="B152" s="14"/>
       <c r="C152" s="15"/>
       <c r="D152" s="6"/>
       <c r="E152" s="16"/>
     </row>
-    <row r="153" spans="1:5">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="14"/>
       <c r="B153" s="14"/>
       <c r="C153" s="15"/>
       <c r="D153" s="6"/>
       <c r="E153" s="16"/>
     </row>
-    <row r="154" spans="1:5">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="14"/>
       <c r="B154" s="14"/>
       <c r="C154" s="15"/>
       <c r="D154" s="6"/>
       <c r="E154" s="16"/>
     </row>
-    <row r="155" spans="1:5">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="14"/>
       <c r="B155" s="14"/>
       <c r="C155" s="15"/>
       <c r="D155" s="6"/>
       <c r="E155" s="16"/>
     </row>
-    <row r="156" spans="1:5">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="14"/>
       <c r="B156" s="14"/>
       <c r="C156" s="15"/>
       <c r="D156" s="6"/>
       <c r="E156" s="16"/>
     </row>
-    <row r="157" spans="1:5">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="14"/>
       <c r="B157" s="14"/>
       <c r="C157" s="15"/>
       <c r="D157" s="6"/>
       <c r="E157" s="16"/>
     </row>
-    <row r="158" spans="1:5">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="14"/>
       <c r="B158" s="14"/>
       <c r="C158" s="15"/>
       <c r="D158" s="6"/>
       <c r="E158" s="16"/>
     </row>
-    <row r="159" spans="1:5">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="14"/>
       <c r="B159" s="14"/>
       <c r="C159" s="15"/>
       <c r="D159" s="6"/>
       <c r="E159" s="16"/>
     </row>
-    <row r="160" spans="1:5">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="14"/>
       <c r="B160" s="14"/>
       <c r="C160" s="15"/>
       <c r="D160" s="6"/>
       <c r="E160" s="16"/>
     </row>
-    <row r="161" spans="1:5">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="14"/>
       <c r="B161" s="14"/>
       <c r="C161" s="15"/>
       <c r="D161" s="6"/>
       <c r="E161" s="16"/>
     </row>
-    <row r="162" spans="1:5">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="14"/>
       <c r="B162" s="14"/>
       <c r="C162" s="15"/>
       <c r="D162" s="6"/>
       <c r="E162" s="16"/>
     </row>
-    <row r="163" spans="1:5">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="14"/>
       <c r="B163" s="14"/>
       <c r="C163" s="15"/>
       <c r="D163" s="6"/>
       <c r="E163" s="16"/>
     </row>
-    <row r="164" spans="1:5">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="14"/>
       <c r="B164" s="14"/>
       <c r="C164" s="15"/>
       <c r="D164" s="6"/>
       <c r="E164" s="16"/>
     </row>
-    <row r="165" spans="1:5">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="14"/>
       <c r="B165" s="14"/>
       <c r="C165" s="15"/>
       <c r="D165" s="6"/>
       <c r="E165" s="16"/>
     </row>
-    <row r="166" spans="1:5">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="14"/>
       <c r="B166" s="14"/>
       <c r="C166" s="15"/>
       <c r="D166" s="6"/>
       <c r="E166" s="16"/>
     </row>
-    <row r="167" spans="1:5">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="14"/>
       <c r="B167" s="14"/>
       <c r="C167" s="15"/>
       <c r="D167" s="6"/>
       <c r="E167" s="16"/>
     </row>
-    <row r="168" spans="1:5">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="14"/>
       <c r="B168" s="14"/>
       <c r="C168" s="15"/>
       <c r="D168" s="6"/>
       <c r="E168" s="16"/>
     </row>
-    <row r="169" spans="1:5">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="14"/>
       <c r="B169" s="14"/>
       <c r="C169" s="15"/>
       <c r="D169" s="6"/>
       <c r="E169" s="16"/>
     </row>
-    <row r="170" spans="1:5">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="14"/>
       <c r="B170" s="14"/>
       <c r="C170" s="15"/>
       <c r="D170" s="6"/>
       <c r="E170" s="16"/>
     </row>
-    <row r="171" spans="1:5">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="14"/>
       <c r="B171" s="14"/>
       <c r="C171" s="15"/>
       <c r="D171" s="6"/>
       <c r="E171" s="16"/>
     </row>
-    <row r="172" spans="1:5">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="14"/>
       <c r="B172" s="14"/>
       <c r="C172" s="15"/>
       <c r="D172" s="6"/>
       <c r="E172" s="16"/>
     </row>
-    <row r="173" spans="1:5">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="14"/>
       <c r="B173" s="14"/>
       <c r="C173" s="15"/>
       <c r="D173" s="6"/>
       <c r="E173" s="16"/>
     </row>
-    <row r="174" spans="1:5">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="14"/>
       <c r="B174" s="14"/>
       <c r="C174" s="15"/>
       <c r="D174" s="6"/>
       <c r="E174" s="16"/>
     </row>
-    <row r="175" spans="1:5">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="14"/>
       <c r="B175" s="14"/>
       <c r="C175" s="15"/>
       <c r="D175" s="6"/>
       <c r="E175" s="16"/>
     </row>
-    <row r="176" spans="1:5">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="14"/>
       <c r="B176" s="14"/>
       <c r="C176" s="15"/>
       <c r="D176" s="6"/>
       <c r="E176" s="16"/>
     </row>
-    <row r="177" spans="1:5">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="14"/>
       <c r="B177" s="14"/>
       <c r="C177" s="15"/>
       <c r="D177" s="6"/>
       <c r="E177" s="16"/>
     </row>
-    <row r="178" spans="1:5">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="14"/>
       <c r="B178" s="14"/>
       <c r="C178" s="15"/>
       <c r="D178" s="6"/>
       <c r="E178" s="16"/>
     </row>
-    <row r="179" spans="1:5">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="14"/>
       <c r="B179" s="14"/>
       <c r="C179" s="15"/>
       <c r="D179" s="6"/>
       <c r="E179" s="16"/>
     </row>
-    <row r="180" spans="1:5">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="14"/>
       <c r="B180" s="14"/>
       <c r="C180" s="15"/>
       <c r="D180" s="6"/>
       <c r="E180" s="16"/>
     </row>
-    <row r="181" spans="1:5">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="14"/>
       <c r="B181" s="14"/>
       <c r="C181" s="15"/>
       <c r="D181" s="6"/>
       <c r="E181" s="16"/>
     </row>
-    <row r="182" spans="1:5">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="14"/>
       <c r="B182" s="14"/>
       <c r="C182" s="15"/>
       <c r="D182" s="6"/>
       <c r="E182" s="16"/>
     </row>
-    <row r="183" spans="1:5">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="14"/>
       <c r="B183" s="14"/>
       <c r="C183" s="15"/>
       <c r="D183" s="6"/>
       <c r="E183" s="16"/>
     </row>
-    <row r="184" spans="1:5">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="14"/>
       <c r="B184" s="14"/>
       <c r="C184" s="15"/>
       <c r="D184" s="6"/>
       <c r="E184" s="16"/>
     </row>
-    <row r="185" spans="1:5">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="14"/>
       <c r="B185" s="14"/>
       <c r="C185" s="15"/>
       <c r="D185" s="6"/>
       <c r="E185" s="16"/>
     </row>
-    <row r="186" spans="1:5">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="14"/>
       <c r="B186" s="14"/>
       <c r="C186" s="15"/>
       <c r="D186" s="6"/>
       <c r="E186" s="16"/>
     </row>
-    <row r="187" spans="1:5">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="14"/>
       <c r="B187" s="14"/>
       <c r="C187" s="15"/>
       <c r="D187" s="6"/>
       <c r="E187" s="16"/>
     </row>
-    <row r="188" spans="1:5">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="14"/>
       <c r="B188" s="14"/>
       <c r="C188" s="15"/>
       <c r="D188" s="6"/>
       <c r="E188" s="16"/>
     </row>
-    <row r="189" spans="1:5">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="14"/>
       <c r="B189" s="14"/>
       <c r="C189" s="15"/>
       <c r="D189" s="6"/>
       <c r="E189" s="16"/>
     </row>
-    <row r="190" spans="1:5">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="14"/>
       <c r="B190" s="14"/>
       <c r="C190" s="15"/>
       <c r="D190" s="6"/>
       <c r="E190" s="16"/>
     </row>
-    <row r="191" spans="1:5">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="14"/>
       <c r="B191" s="14"/>
       <c r="C191" s="15"/>
       <c r="D191" s="6"/>
       <c r="E191" s="16"/>
     </row>
-    <row r="192" spans="1:5">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="14"/>
       <c r="B192" s="14"/>
       <c r="C192" s="15"/>
       <c r="D192" s="6"/>
       <c r="E192" s="16"/>
     </row>
-    <row r="193" spans="1:5">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="14"/>
       <c r="B193" s="14"/>
       <c r="C193" s="15"/>
       <c r="D193" s="6"/>
       <c r="E193" s="16"/>
     </row>
-    <row r="194" spans="1:5">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="14"/>
       <c r="B194" s="14"/>
       <c r="C194" s="15"/>
       <c r="D194" s="6"/>
       <c r="E194" s="16"/>
     </row>
-    <row r="195" spans="1:5">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="14"/>
       <c r="B195" s="14"/>
       <c r="C195" s="15"/>
       <c r="D195" s="6"/>
       <c r="E195" s="16"/>
     </row>
-    <row r="196" spans="1:5">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="14"/>
       <c r="B196" s="14"/>
       <c r="C196" s="15"/>
       <c r="D196" s="6"/>
       <c r="E196" s="16"/>
     </row>
-    <row r="197" spans="1:5">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="14"/>
       <c r="B197" s="14"/>
       <c r="C197" s="15"/>
       <c r="D197" s="6"/>
       <c r="E197" s="16"/>
     </row>
-    <row r="198" spans="1:5">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="14"/>
       <c r="B198" s="14"/>
       <c r="C198" s="15"/>
       <c r="D198" s="6"/>
       <c r="E198" s="16"/>
     </row>
-    <row r="199" spans="1:5">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="14"/>
       <c r="B199" s="14"/>
       <c r="C199" s="15"/>
       <c r="D199" s="6"/>
       <c r="E199" s="16"/>
     </row>
-    <row r="200" spans="1:5">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="14"/>
       <c r="B200" s="14"/>
       <c r="C200" s="15"/>
       <c r="D200" s="6"/>
       <c r="E200" s="16"/>
     </row>
-    <row r="201" spans="1:5">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="14"/>
       <c r="B201" s="14"/>
       <c r="C201" s="15"/>
       <c r="D201" s="6"/>
       <c r="E201" s="16"/>
     </row>
-    <row r="202" spans="1:5">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="14"/>
       <c r="B202" s="14"/>
       <c r="C202" s="15"/>
       <c r="D202" s="6"/>
       <c r="E202" s="16"/>
     </row>
-    <row r="203" spans="1:5">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="14"/>
       <c r="B203" s="14"/>
       <c r="C203" s="15"/>
       <c r="D203" s="6"/>
       <c r="E203" s="16"/>
     </row>
-    <row r="204" spans="1:5">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="14"/>
       <c r="B204" s="14"/>
       <c r="C204" s="15"/>
       <c r="D204" s="6"/>
       <c r="E204" s="16"/>
     </row>
-    <row r="205" spans="1:5">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="14"/>
       <c r="B205" s="14"/>
       <c r="C205" s="15"/>
       <c r="D205" s="6"/>
       <c r="E205" s="16"/>
     </row>
-    <row r="206" spans="1:5">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="14"/>
       <c r="B206" s="14"/>
       <c r="C206" s="15"/>
       <c r="D206" s="6"/>
       <c r="E206" s="16"/>
     </row>
-    <row r="207" spans="1:5">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="14"/>
       <c r="B207" s="14"/>
       <c r="C207" s="15"/>
       <c r="D207" s="6"/>
       <c r="E207" s="16"/>
     </row>
-    <row r="208" spans="1:5">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="14"/>
       <c r="B208" s="14"/>
       <c r="C208" s="15"/>
       <c r="D208" s="6"/>
       <c r="E208" s="16"/>
     </row>
-    <row r="209" spans="3:3" ht="21">
+    <row r="209" spans="3:3" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="C209" s="15" t="s">
         <v>10</v>
       </c>
@@ -2262,7 +2313,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:IV41"/>
   <sheetViews>
@@ -2270,16 +2321,16 @@
       <selection activeCell="CB29" sqref="CB29:CT29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="32.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.5546875" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="32.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" s="5" customFormat="1">
+    <row r="2" spans="1:13" s="5" customFormat="1" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
@@ -2296,17 +2347,17 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" s="7" customFormat="1" ht="10.5">
+    <row r="3" spans="1:13" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="C3" s="8"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
     </row>
-    <row r="4" spans="1:13" s="7" customFormat="1" ht="10.5">
+    <row r="4" spans="1:13" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="C4" s="8"/>
       <c r="D4" s="9"/>
       <c r="E4" s="10"/>
     </row>
-    <row r="5" spans="1:13" s="9" customFormat="1" ht="21">
+    <row r="5" spans="1:13" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>0</v>
       </c>
@@ -2323,7 +2374,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="7" customFormat="1" ht="10.5">
+    <row r="6" spans="1:13" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>5</v>
       </c>
@@ -2332,12 +2383,12 @@
       <c r="D6" s="6"/>
       <c r="E6" s="16"/>
     </row>
-    <row r="7" spans="1:13" s="7" customFormat="1" ht="10.5">
+    <row r="7" spans="1:13" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="C7" s="15"/>
       <c r="D7" s="6"/>
       <c r="E7" s="16"/>
     </row>
-    <row r="8" spans="1:13" s="7" customFormat="1" ht="52.5">
+    <row r="8" spans="1:13" s="7" customFormat="1" ht="40.799999999999997" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>8</v>
       </c>
@@ -2351,7 +2402,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="7" customFormat="1" ht="10.5">
+    <row r="9" spans="1:13" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>5</v>
       </c>
@@ -2365,7 +2416,7 @@
       <c r="E9" s="16"/>
       <c r="F9" s="18"/>
     </row>
-    <row r="10" spans="1:13" s="7" customFormat="1" ht="52.5">
+    <row r="10" spans="1:13" s="7" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>5</v>
       </c>
@@ -2381,7 +2432,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="7" customFormat="1" ht="10.5">
+    <row r="11" spans="1:13" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
@@ -2392,7 +2443,7 @@
       <c r="D11" s="6"/>
       <c r="E11" s="16"/>
     </row>
-    <row r="12" spans="1:13" s="7" customFormat="1" ht="21">
+    <row r="12" spans="1:13" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>8</v>
       </c>
@@ -2403,7 +2454,7 @@
       <c r="D12" s="6"/>
       <c r="E12" s="16"/>
     </row>
-    <row r="13" spans="1:13" s="7" customFormat="1" ht="10.5">
+    <row r="13" spans="1:13" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>5</v>
       </c>
@@ -2416,7 +2467,7 @@
       <c r="D13" s="6"/>
       <c r="E13" s="16"/>
     </row>
-    <row r="14" spans="1:13" s="7" customFormat="1" ht="10.5">
+    <row r="14" spans="1:13" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>5</v>
       </c>
@@ -2430,7 +2481,7 @@
       <c r="E14" s="16"/>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:13" s="7" customFormat="1" ht="10.5">
+    <row r="15" spans="1:13" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="25" t="s">
         <v>18</v>
@@ -2442,7 +2493,7 @@
       <c r="E15" s="16"/>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:13" s="7" customFormat="1" ht="10.5">
+    <row r="16" spans="1:13" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>5</v>
       </c>
@@ -2455,7 +2506,7 @@
       <c r="D16" s="6"/>
       <c r="E16" s="16"/>
     </row>
-    <row r="17" spans="1:256" s="7" customFormat="1" ht="21">
+    <row r="17" spans="1:256" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>5</v>
       </c>
@@ -2466,7 +2517,7 @@
       <c r="D17" s="6"/>
       <c r="E17" s="16"/>
     </row>
-    <row r="18" spans="1:256" s="7" customFormat="1" ht="10.5">
+    <row r="18" spans="1:256" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
@@ -2479,7 +2530,7 @@
       <c r="D18" s="6"/>
       <c r="E18" s="16"/>
     </row>
-    <row r="19" spans="1:256" s="7" customFormat="1" ht="10.5">
+    <row r="19" spans="1:256" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>5</v>
       </c>
@@ -2492,7 +2543,7 @@
       <c r="D19" s="6"/>
       <c r="E19" s="16"/>
     </row>
-    <row r="20" spans="1:256" s="7" customFormat="1" ht="10.5">
+    <row r="20" spans="1:256" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>5</v>
       </c>
@@ -2505,7 +2556,7 @@
       <c r="D20" s="6"/>
       <c r="E20" s="16"/>
     </row>
-    <row r="21" spans="1:256" s="7" customFormat="1" ht="11.25" customHeight="1">
+    <row r="21" spans="1:256" s="7" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>5</v>
       </c>
@@ -2516,7 +2567,7 @@
       <c r="D21" s="6"/>
       <c r="E21" s="16"/>
     </row>
-    <row r="22" spans="1:256" s="7" customFormat="1" ht="10.5">
+    <row r="22" spans="1:256" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>5</v>
       </c>
@@ -2529,7 +2580,7 @@
       <c r="D22" s="6"/>
       <c r="E22" s="16"/>
     </row>
-    <row r="23" spans="1:256" s="7" customFormat="1" ht="21" customHeight="1">
+    <row r="23" spans="1:256" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>8</v>
       </c>
@@ -2542,7 +2593,7 @@
       <c r="D23" s="6"/>
       <c r="E23" s="16"/>
     </row>
-    <row r="24" spans="1:256" s="7" customFormat="1" ht="18" customHeight="1">
+    <row r="24" spans="1:256" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="14" t="s">
         <v>34</v>
@@ -2553,7 +2604,7 @@
       <c r="D24" s="6"/>
       <c r="E24" s="16"/>
     </row>
-    <row r="25" spans="1:256" s="7" customFormat="1" ht="15.75" customHeight="1">
+    <row r="25" spans="1:256" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="14" t="s">
         <v>36</v>
@@ -2564,7 +2615,7 @@
       <c r="D25" s="6"/>
       <c r="E25" s="16"/>
     </row>
-    <row r="26" spans="1:256" s="7" customFormat="1" ht="15.75" customHeight="1">
+    <row r="26" spans="1:256" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="14" t="s">
         <v>22</v>
@@ -2575,7 +2626,7 @@
       <c r="D26" s="6"/>
       <c r="E26" s="16"/>
     </row>
-    <row r="27" spans="1:256" s="7" customFormat="1" ht="14.25" customHeight="1">
+    <row r="27" spans="1:256" s="7" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>
       <c r="B27" s="14" t="s">
         <v>37</v>
@@ -2586,7 +2637,7 @@
       <c r="D27" s="6"/>
       <c r="E27" s="16"/>
     </row>
-    <row r="28" spans="1:256" s="7" customFormat="1" ht="15" customHeight="1">
+    <row r="28" spans="1:256" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14"/>
       <c r="B28" s="14" t="s">
         <v>38</v>
@@ -2597,7 +2648,7 @@
       <c r="D28" s="6"/>
       <c r="E28" s="16"/>
     </row>
-    <row r="29" spans="1:256" s="7" customFormat="1" ht="14.25" customHeight="1">
+    <row r="29" spans="1:256" s="7" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
       <c r="B29" s="14" t="s">
         <v>39</v>
@@ -2859,7 +2910,7 @@
       <c r="IU29" s="14"/>
       <c r="IV29" s="14"/>
     </row>
-    <row r="30" spans="1:256" s="7" customFormat="1" ht="21">
+    <row r="30" spans="1:256" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>5</v>
       </c>
@@ -2876,7 +2927,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:256" s="7" customFormat="1" ht="10.5">
+    <row r="31" spans="1:256" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A31" s="14"/>
       <c r="B31" s="14"/>
       <c r="C31" s="19" t="s">
@@ -2885,7 +2936,7 @@
       <c r="D31" s="6"/>
       <c r="E31" s="16"/>
     </row>
-    <row r="32" spans="1:256" s="7" customFormat="1" ht="21">
+    <row r="32" spans="1:256" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A32" s="14"/>
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
@@ -2894,7 +2945,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="7" customFormat="1" ht="10.5">
+    <row r="33" spans="1:5" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A33" s="14"/>
       <c r="B33" s="14"/>
       <c r="C33" s="19" t="s">
@@ -2903,7 +2954,7 @@
       <c r="D33" s="6"/>
       <c r="E33" s="16"/>
     </row>
-    <row r="34" spans="1:5" s="7" customFormat="1" ht="21">
+    <row r="34" spans="1:5" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A34" s="14"/>
       <c r="B34" s="14"/>
       <c r="C34" s="15"/>
@@ -2912,7 +2963,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="7" customFormat="1" ht="10.5">
+    <row r="35" spans="1:5" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A35" s="14"/>
       <c r="B35" s="14"/>
       <c r="C35" s="19" t="s">
@@ -2921,7 +2972,7 @@
       <c r="D35" s="6"/>
       <c r="E35" s="16"/>
     </row>
-    <row r="36" spans="1:5" s="7" customFormat="1" ht="21">
+    <row r="36" spans="1:5" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A36" s="14"/>
       <c r="B36" s="14"/>
       <c r="C36" s="15"/>
@@ -2930,7 +2981,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="7" customFormat="1" ht="10.5">
+    <row r="37" spans="1:5" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="19" t="s">
@@ -2939,28 +2990,28 @@
       <c r="D37" s="6"/>
       <c r="E37" s="16"/>
     </row>
-    <row r="38" spans="1:5" s="7" customFormat="1" ht="10.5">
+    <row r="38" spans="1:5" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A38" s="14"/>
       <c r="B38" s="14"/>
       <c r="C38" s="15"/>
       <c r="D38" s="6"/>
       <c r="E38" s="16"/>
     </row>
-    <row r="39" spans="1:5" s="7" customFormat="1" ht="10.5">
+    <row r="39" spans="1:5" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A39" s="14"/>
       <c r="B39" s="14"/>
       <c r="C39" s="15"/>
       <c r="D39" s="6"/>
       <c r="E39" s="16"/>
     </row>
-    <row r="40" spans="1:5" s="7" customFormat="1" ht="10.5">
+    <row r="40" spans="1:5" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A40" s="14"/>
       <c r="B40" s="14"/>
       <c r="C40" s="15"/>
       <c r="D40" s="6"/>
       <c r="E40" s="16"/>
     </row>
-    <row r="41" spans="1:5" s="7" customFormat="1" ht="10.5">
+    <row r="41" spans="1:5" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A41" s="14"/>
       <c r="B41" s="14"/>
       <c r="C41" s="15"/>
@@ -2975,24 +3026,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="28.28515625" customWidth="1"/>
+    <col min="1" max="1" width="22.88671875" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" s="5" customFormat="1">
+    <row r="2" spans="1:13" s="5" customFormat="1" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>32</v>
       </c>
@@ -3009,17 +3060,17 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" s="7" customFormat="1" ht="10.5">
+    <row r="3" spans="1:13" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="C3" s="8"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
     </row>
-    <row r="4" spans="1:13" s="7" customFormat="1" ht="10.5">
+    <row r="4" spans="1:13" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="C4" s="8"/>
       <c r="D4" s="9"/>
       <c r="E4" s="10"/>
     </row>
-    <row r="5" spans="1:13" s="9" customFormat="1" ht="21">
+    <row r="5" spans="1:13" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>0</v>
       </c>
@@ -3036,7 +3087,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="7" customFormat="1" ht="10.5">
+    <row r="6" spans="1:13" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>5</v>
       </c>
@@ -3045,12 +3096,12 @@
       <c r="D6" s="6"/>
       <c r="E6" s="16"/>
     </row>
-    <row r="7" spans="1:13" s="7" customFormat="1" ht="10.5">
+    <row r="7" spans="1:13" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="C7" s="15"/>
       <c r="D7" s="6"/>
       <c r="E7" s="16"/>
     </row>
-    <row r="8" spans="1:13" s="7" customFormat="1" ht="52.5">
+    <row r="8" spans="1:13" s="7" customFormat="1" ht="40.799999999999997" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>8</v>
       </c>
@@ -3064,7 +3115,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="7" customFormat="1" ht="10.5">
+    <row r="9" spans="1:13" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>5</v>
       </c>
@@ -3078,7 +3129,7 @@
       <c r="E9" s="16"/>
       <c r="F9" s="18"/>
     </row>
-    <row r="10" spans="1:13" s="7" customFormat="1" ht="52.5">
+    <row r="10" spans="1:13" s="7" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>5</v>
       </c>
@@ -3094,7 +3145,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="7" customFormat="1" ht="10.5">
+    <row r="11" spans="1:13" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
@@ -3105,7 +3156,7 @@
       <c r="D11" s="6"/>
       <c r="E11" s="16"/>
     </row>
-    <row r="12" spans="1:13" s="7" customFormat="1" ht="21">
+    <row r="12" spans="1:13" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>8</v>
       </c>
@@ -3116,7 +3167,7 @@
       <c r="D12" s="6"/>
       <c r="E12" s="16"/>
     </row>
-    <row r="13" spans="1:13" s="7" customFormat="1">
+    <row r="13" spans="1:13" s="7" customFormat="1" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="24" t="s">
         <v>41</v>
@@ -3127,7 +3178,7 @@
       <c r="D13" s="6"/>
       <c r="E13" s="16"/>
     </row>
-    <row r="14" spans="1:13" s="7" customFormat="1">
+    <row r="14" spans="1:13" s="7" customFormat="1" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>5</v>
       </c>
@@ -3140,7 +3191,7 @@
       <c r="D14" s="6"/>
       <c r="E14" s="16"/>
     </row>
-    <row r="15" spans="1:13" s="7" customFormat="1">
+    <row r="15" spans="1:13" s="7" customFormat="1" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>5</v>
       </c>
@@ -3154,7 +3205,7 @@
       <c r="E15" s="16"/>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:13" s="7" customFormat="1">
+    <row r="16" spans="1:13" s="7" customFormat="1" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>5</v>
       </c>
@@ -3167,7 +3218,7 @@
       <c r="D16" s="6"/>
       <c r="E16" s="16"/>
     </row>
-    <row r="17" spans="1:5" s="7" customFormat="1" ht="21">
+    <row r="17" spans="1:5" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>5</v>
       </c>
@@ -3178,7 +3229,7 @@
       <c r="D17" s="6"/>
       <c r="E17" s="16"/>
     </row>
-    <row r="18" spans="1:5" s="7" customFormat="1" ht="10.5">
+    <row r="18" spans="1:5" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
@@ -3191,7 +3242,7 @@
       <c r="D18" s="6"/>
       <c r="E18" s="16"/>
     </row>
-    <row r="19" spans="1:5" s="7" customFormat="1" ht="10.5">
+    <row r="19" spans="1:5" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>5</v>
       </c>
@@ -3204,7 +3255,7 @@
       <c r="D19" s="6"/>
       <c r="E19" s="16"/>
     </row>
-    <row r="20" spans="1:5" s="7" customFormat="1" ht="10.5">
+    <row r="20" spans="1:5" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>5</v>
       </c>
@@ -3217,7 +3268,7 @@
       <c r="D20" s="6"/>
       <c r="E20" s="16"/>
     </row>
-    <row r="21" spans="1:5" s="7" customFormat="1" ht="10.5">
+    <row r="21" spans="1:5" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>5</v>
       </c>
@@ -3228,7 +3279,7 @@
       <c r="D21" s="6"/>
       <c r="E21" s="16"/>
     </row>
-    <row r="22" spans="1:5" s="7" customFormat="1" ht="10.5">
+    <row r="22" spans="1:5" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="15" t="s">
         <v>25</v>
@@ -3239,7 +3290,7 @@
       <c r="D22" s="6"/>
       <c r="E22" s="16"/>
     </row>
-    <row r="23" spans="1:5" s="7" customFormat="1" ht="31.5">
+    <row r="23" spans="1:5" s="7" customFormat="1" ht="30.6" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>8</v>
       </c>
@@ -3250,7 +3301,7 @@
       <c r="D23" s="6"/>
       <c r="E23" s="16"/>
     </row>
-    <row r="24" spans="1:5" s="7" customFormat="1" ht="10.5">
+    <row r="24" spans="1:5" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="14" t="s">
         <v>34</v>
@@ -3261,7 +3312,7 @@
       <c r="D24" s="6"/>
       <c r="E24" s="16"/>
     </row>
-    <row r="25" spans="1:5" s="7" customFormat="1" ht="10.5">
+    <row r="25" spans="1:5" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="14" t="s">
         <v>36</v>
@@ -3272,7 +3323,7 @@
       <c r="D25" s="6"/>
       <c r="E25" s="16"/>
     </row>
-    <row r="26" spans="1:5" s="7" customFormat="1" ht="10.5">
+    <row r="26" spans="1:5" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="14" t="s">
         <v>22</v>
@@ -3283,7 +3334,7 @@
       <c r="D26" s="6"/>
       <c r="E26" s="16"/>
     </row>
-    <row r="27" spans="1:5" s="7" customFormat="1" ht="10.5">
+    <row r="27" spans="1:5" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>
       <c r="B27" s="14" t="s">
         <v>37</v>
@@ -3294,7 +3345,7 @@
       <c r="D27" s="6"/>
       <c r="E27" s="16"/>
     </row>
-    <row r="28" spans="1:5" s="7" customFormat="1" ht="10.5">
+    <row r="28" spans="1:5" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A28" s="14"/>
       <c r="B28" s="14" t="s">
         <v>38</v>
@@ -3305,7 +3356,7 @@
       <c r="D28" s="6"/>
       <c r="E28" s="16"/>
     </row>
-    <row r="29" spans="1:5" s="7" customFormat="1" ht="10.5">
+    <row r="29" spans="1:5" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
       <c r="B29" s="14" t="s">
         <v>39</v>
@@ -3316,7 +3367,7 @@
       <c r="D29" s="6"/>
       <c r="E29" s="16"/>
     </row>
-    <row r="30" spans="1:5" s="7" customFormat="1" ht="31.5">
+    <row r="30" spans="1:5" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>5</v>
       </c>
@@ -3333,7 +3384,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="7" customFormat="1" ht="10.5">
+    <row r="31" spans="1:5" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A31" s="14"/>
       <c r="B31" s="14"/>
       <c r="C31" s="19" t="s">
@@ -3342,7 +3393,7 @@
       <c r="D31" s="6"/>
       <c r="E31" s="16"/>
     </row>
-    <row r="32" spans="1:5" s="7" customFormat="1" ht="31.5">
+    <row r="32" spans="1:5" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A32" s="14"/>
       <c r="B32" s="14"/>
       <c r="C32" s="15" t="s">
@@ -3355,7 +3406,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="7" customFormat="1" ht="10.5">
+    <row r="33" spans="1:5" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A33" s="14"/>
       <c r="B33" s="14"/>
       <c r="C33" s="19" t="s">
@@ -3364,7 +3415,7 @@
       <c r="D33" s="6"/>
       <c r="E33" s="16"/>
     </row>
-    <row r="34" spans="1:5" s="7" customFormat="1" ht="31.5">
+    <row r="34" spans="1:5" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A34" s="14"/>
       <c r="B34" s="14"/>
       <c r="C34" s="15" t="s">
@@ -3377,7 +3428,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="7" customFormat="1" ht="10.5">
+    <row r="35" spans="1:5" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A35" s="14"/>
       <c r="B35" s="14"/>
       <c r="C35" s="19" t="s">
@@ -3386,7 +3437,7 @@
       <c r="D35" s="6"/>
       <c r="E35" s="16"/>
     </row>
-    <row r="36" spans="1:5" s="7" customFormat="1" ht="31.5">
+    <row r="36" spans="1:5" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A36" s="14"/>
       <c r="B36" s="14"/>
       <c r="C36" s="15" t="s">
@@ -3399,7 +3450,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="7" customFormat="1" ht="10.5">
+    <row r="37" spans="1:5" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="19" t="s">
@@ -3408,7 +3459,7 @@
       <c r="D37" s="6"/>
       <c r="E37" s="16"/>
     </row>
-    <row r="38" spans="1:5" s="7" customFormat="1" ht="21">
+    <row r="38" spans="1:5" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A38" s="14"/>
       <c r="B38" s="14"/>
       <c r="C38" s="15" t="s">
@@ -3421,7 +3472,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="7" customFormat="1" ht="10.5">
+    <row r="39" spans="1:5" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A39" s="14"/>
       <c r="B39" s="14"/>
       <c r="C39" s="19" t="s">
@@ -3430,7 +3481,7 @@
       <c r="D39" s="6"/>
       <c r="E39" s="16"/>
     </row>
-    <row r="40" spans="1:5" s="7" customFormat="1" ht="21">
+    <row r="40" spans="1:5" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A40" s="14"/>
       <c r="B40" s="14"/>
       <c r="C40" s="15" t="s">
@@ -3443,7 +3494,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="7" customFormat="1" ht="10.5">
+    <row r="41" spans="1:5" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A41" s="14"/>
       <c r="B41" s="14"/>
       <c r="C41" s="19" t="s">
@@ -3452,7 +3503,7 @@
       <c r="D41" s="6"/>
       <c r="E41" s="16"/>
     </row>
-    <row r="42" spans="1:5" s="7" customFormat="1" ht="25.5" customHeight="1">
+    <row r="42" spans="1:5" s="7" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="14"/>
       <c r="B42" s="14"/>
       <c r="C42" s="15" t="s">
@@ -3465,7 +3516,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:5" s="7" customFormat="1" ht="10.5">
+    <row r="43" spans="1:5" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A43" s="14"/>
       <c r="B43" s="14"/>
       <c r="C43" s="19" t="s">
@@ -3474,7 +3525,7 @@
       <c r="D43" s="6"/>
       <c r="E43" s="16"/>
     </row>
-    <row r="44" spans="1:5" s="7" customFormat="1" ht="10.5">
+    <row r="44" spans="1:5" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.25">
       <c r="A44" s="14"/>
       <c r="B44" s="14"/>
       <c r="C44" s="15"/>
@@ -3487,4 +3538,16 @@
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6EFBDA3-B083-44EF-98F2-314E344BF368}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>